<commit_message>
Apply cosmetic changes to plots: x-axis in seconds, p5/p10 default lines with legends, detailed title dates, and station completeness color gradient. Update README examples.
</commit_message>
<xml_diff>
--- a/psd_results/BK_PSD_50vs1_p50.xlsx
+++ b/psd_results/BK_PSD_50vs1_p50.xlsx
@@ -468,128 +468,128 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BL67</t>
+          <t>BKS</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-133</v>
+        <v>-160</v>
       </c>
       <c r="C3" t="n">
-        <v>-130</v>
+        <v>-131</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>BRK</t>
+          <t>BL67</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-147</v>
+        <v>-133</v>
       </c>
       <c r="C4" t="n">
-        <v>-134</v>
+        <v>-130</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CMB</t>
+          <t>BRK</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-160</v>
+        <v>-147</v>
       </c>
       <c r="C5" t="n">
-        <v>-153</v>
+        <v>-134</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>FARB</t>
+          <t>CMB</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-136</v>
+        <v>-160</v>
       </c>
       <c r="C6" t="n">
-        <v>-126</v>
+        <v>-153</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>HATC</t>
+          <t>FARB</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-163</v>
+        <v>-136</v>
       </c>
       <c r="C7" t="n">
-        <v>-140</v>
+        <v>-126</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>HOPS</t>
+          <t>HATC</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-158</v>
+        <v>-163</v>
       </c>
       <c r="C8" t="n">
-        <v>-133</v>
+        <v>-140</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>JCC</t>
+          <t>HOPS</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-169</v>
+        <v>-158</v>
       </c>
       <c r="C9" t="n">
-        <v>-129</v>
+        <v>-133</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>MCCM</t>
+          <t>JCC</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-154</v>
+        <v>-169</v>
       </c>
       <c r="C10" t="n">
-        <v>-125</v>
+        <v>-129</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>MHC</t>
+          <t>MCCM</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>-154</v>
       </c>
       <c r="C11" t="n">
-        <v>-140</v>
+        <v>-125</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>MNRC</t>
+          <t>MHC</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-159</v>
+        <v>-154</v>
       </c>
       <c r="C12" t="n">
         <v>-140</v>
@@ -598,157 +598,157 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>MOD</t>
+          <t>MNRC</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-157</v>
+        <v>-159</v>
       </c>
       <c r="C13" t="n">
-        <v>-148</v>
+        <v>-140</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ORV</t>
+          <t>MOD</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-168</v>
+        <v>-157</v>
       </c>
       <c r="C14" t="n">
-        <v>-152</v>
+        <v>-148</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>PACP</t>
+          <t>ORV</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-150</v>
+        <v>-168</v>
       </c>
       <c r="C15" t="n">
-        <v>-137</v>
+        <v>-152</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>PKD</t>
+          <t>PACP</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-153</v>
+        <v>-150</v>
       </c>
       <c r="C16" t="n">
-        <v>-136</v>
+        <v>-137</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>SAO</t>
+          <t>PKD</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-154</v>
+        <v>-153</v>
       </c>
       <c r="C17" t="n">
-        <v>-137</v>
+        <v>-136</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>SCZ</t>
+          <t>SAO</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-166</v>
+        <v>-154</v>
       </c>
       <c r="C18" t="n">
-        <v>-143</v>
+        <v>-137</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>TCHL</t>
+          <t>SCZ</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-158</v>
+        <v>-166</v>
       </c>
       <c r="C19" t="n">
-        <v>-133</v>
+        <v>-143</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>THIS</t>
+          <t>TCHL</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-190</v>
+        <v>-158</v>
       </c>
       <c r="C20" t="n">
-        <v>-134</v>
+        <v>-133</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>TSCN</t>
+          <t>THIS</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-150</v>
+        <v>-190</v>
       </c>
       <c r="C21" t="n">
-        <v>-128</v>
+        <v>-134</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>VAK</t>
+          <t>TSCN</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-148</v>
+        <v>-150</v>
       </c>
       <c r="C22" t="n">
-        <v>-126</v>
+        <v>-128</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>WENL</t>
+          <t>VAK</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>-192</v>
+        <v>-148</v>
       </c>
       <c r="C23" t="n">
-        <v>-175</v>
+        <v>-126</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>YBH</t>
+          <t>WENL</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>-173</v>
+        <v>-192</v>
       </c>
       <c r="C24" t="n">
-        <v>-150</v>
+        <v>-175</v>
       </c>
     </row>
     <row r="25">
@@ -816,11 +816,11 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BL67</t>
+          <t>BKS</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-132</v>
+        <v>-159</v>
       </c>
       <c r="C3" t="n">
         <v>-130</v>
@@ -829,115 +829,115 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>BRK</t>
+          <t>BL67</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-152</v>
+        <v>-132</v>
       </c>
       <c r="C4" t="n">
-        <v>-134</v>
+        <v>-130</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CMB</t>
+          <t>BRK</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-159</v>
+        <v>-152</v>
       </c>
       <c r="C5" t="n">
-        <v>-153</v>
+        <v>-134</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>FARB</t>
+          <t>CMB</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-137</v>
+        <v>-159</v>
       </c>
       <c r="C6" t="n">
-        <v>-126</v>
+        <v>-153</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>HATC</t>
+          <t>FARB</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-163</v>
+        <v>-137</v>
       </c>
       <c r="C7" t="n">
-        <v>-142</v>
+        <v>-126</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>HOPS</t>
+          <t>HATC</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-158</v>
+        <v>-163</v>
       </c>
       <c r="C8" t="n">
-        <v>-133</v>
+        <v>-142</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>JCC</t>
+          <t>HOPS</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-170</v>
+        <v>-158</v>
       </c>
       <c r="C9" t="n">
-        <v>-130</v>
+        <v>-133</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>MCCM</t>
+          <t>JCC</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-154</v>
+        <v>-170</v>
       </c>
       <c r="C10" t="n">
-        <v>-126</v>
+        <v>-130</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>MHC</t>
+          <t>MCCM</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-150</v>
+        <v>-154</v>
       </c>
       <c r="C11" t="n">
-        <v>-139</v>
+        <v>-126</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>MNRC</t>
+          <t>MHC</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-160</v>
+        <v>-150</v>
       </c>
       <c r="C12" t="n">
         <v>-139</v>
@@ -946,50 +946,50 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>MOD</t>
+          <t>MNRC</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-161</v>
+        <v>-160</v>
       </c>
       <c r="C13" t="n">
-        <v>-150</v>
+        <v>-139</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ORV</t>
+          <t>MOD</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-170</v>
+        <v>-161</v>
       </c>
       <c r="C14" t="n">
-        <v>-152</v>
+        <v>-150</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>PACP</t>
+          <t>ORV</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-151</v>
+        <v>-170</v>
       </c>
       <c r="C15" t="n">
-        <v>-137</v>
+        <v>-152</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>PKD</t>
+          <t>PACP</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-154</v>
+        <v>-151</v>
       </c>
       <c r="C16" t="n">
         <v>-137</v>
@@ -998,11 +998,11 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>SAO</t>
+          <t>PKD</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-157</v>
+        <v>-154</v>
       </c>
       <c r="C17" t="n">
         <v>-137</v>
@@ -1011,92 +1011,92 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>SCZ</t>
+          <t>SAO</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-156</v>
+        <v>-157</v>
       </c>
       <c r="C18" t="n">
-        <v>-142</v>
+        <v>-137</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>TCHL</t>
+          <t>SCZ</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-158</v>
+        <v>-156</v>
       </c>
       <c r="C19" t="n">
-        <v>-135</v>
+        <v>-142</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>THIS</t>
+          <t>TCHL</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-148</v>
+        <v>-158</v>
       </c>
       <c r="C20" t="n">
-        <v>-134</v>
+        <v>-135</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>TSCN</t>
+          <t>THIS</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-149</v>
+        <v>-148</v>
       </c>
       <c r="C21" t="n">
-        <v>-129</v>
+        <v>-134</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>VAK</t>
+          <t>TSCN</t>
         </is>
       </c>
       <c r="B22" t="n">
         <v>-149</v>
       </c>
       <c r="C22" t="n">
-        <v>-126</v>
+        <v>-129</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>WENL</t>
+          <t>VAK</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>-178</v>
+        <v>-149</v>
       </c>
       <c r="C23" t="n">
-        <v>-168</v>
+        <v>-126</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>YBH</t>
+          <t>WENL</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>-175</v>
+        <v>-178</v>
       </c>
       <c r="C24" t="n">
-        <v>-151</v>
+        <v>-168</v>
       </c>
     </row>
     <row r="25">
@@ -1164,154 +1164,154 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BL67</t>
+          <t>BKS</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-157</v>
+        <v>-178</v>
       </c>
       <c r="C3" t="n">
-        <v>-133</v>
+        <v>-134</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>BRK</t>
+          <t>BL67</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-170</v>
+        <v>-157</v>
       </c>
       <c r="C4" t="n">
-        <v>-134</v>
+        <v>-133</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CMB</t>
+          <t>BRK</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-179</v>
+        <v>-170</v>
       </c>
       <c r="C5" t="n">
-        <v>-154</v>
+        <v>-134</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>FARB</t>
+          <t>CMB</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-157</v>
+        <v>-179</v>
       </c>
       <c r="C6" t="n">
-        <v>-125</v>
+        <v>-154</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>HATC</t>
+          <t>FARB</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-176</v>
+        <v>-157</v>
       </c>
       <c r="C7" t="n">
-        <v>-138</v>
+        <v>-125</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>HOPS</t>
+          <t>HATC</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-178</v>
+        <v>-176</v>
       </c>
       <c r="C8" t="n">
-        <v>-135</v>
+        <v>-138</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>JCC</t>
+          <t>HOPS</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>-178</v>
       </c>
       <c r="C9" t="n">
-        <v>-128</v>
+        <v>-135</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>MCCM</t>
+          <t>JCC</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>-178</v>
       </c>
       <c r="C10" t="n">
-        <v>-127</v>
+        <v>-128</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>MHC</t>
+          <t>MCCM</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-176</v>
+        <v>-178</v>
       </c>
       <c r="C11" t="n">
-        <v>-143</v>
+        <v>-127</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>MNRC</t>
+          <t>MHC</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>-176</v>
       </c>
       <c r="C12" t="n">
-        <v>-140</v>
+        <v>-143</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>MOD</t>
+          <t>MNRC</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-177</v>
+        <v>-176</v>
       </c>
       <c r="C13" t="n">
-        <v>-152</v>
+        <v>-140</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ORV</t>
+          <t>MOD</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-180</v>
+        <v>-177</v>
       </c>
       <c r="C14" t="n">
         <v>-152</v>
@@ -1320,131 +1320,131 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>PACP</t>
+          <t>ORV</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-170</v>
+        <v>-180</v>
       </c>
       <c r="C15" t="n">
-        <v>-143</v>
+        <v>-152</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>PKD</t>
+          <t>PACP</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-172</v>
+        <v>-170</v>
       </c>
       <c r="C16" t="n">
-        <v>-140</v>
+        <v>-143</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>SAO</t>
+          <t>PKD</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-177</v>
+        <v>-172</v>
       </c>
       <c r="C17" t="n">
-        <v>-139</v>
+        <v>-140</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>SCZ</t>
+          <t>SAO</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-170</v>
+        <v>-177</v>
       </c>
       <c r="C18" t="n">
-        <v>-142</v>
+        <v>-139</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>TCHL</t>
+          <t>SCZ</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-162</v>
+        <v>-170</v>
       </c>
       <c r="C19" t="n">
-        <v>-148</v>
+        <v>-142</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>THIS</t>
+          <t>TCHL</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-177</v>
+        <v>-162</v>
       </c>
       <c r="C20" t="n">
-        <v>-159</v>
+        <v>-148</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>TSCN</t>
+          <t>THIS</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-170</v>
+        <v>-177</v>
       </c>
       <c r="C21" t="n">
-        <v>-133</v>
+        <v>-159</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>VAK</t>
+          <t>TSCN</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-168</v>
+        <v>-170</v>
       </c>
       <c r="C22" t="n">
-        <v>-131</v>
+        <v>-133</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>WENL</t>
+          <t>VAK</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>-191</v>
+        <v>-168</v>
       </c>
       <c r="C23" t="n">
-        <v>-180</v>
+        <v>-131</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>YBH</t>
+          <t>WENL</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>-177</v>
+        <v>-191</v>
       </c>
       <c r="C24" t="n">
-        <v>-150</v>
+        <v>-180</v>
       </c>
     </row>
     <row r="25">

</xml_diff>